<commit_message>
Updated silhouette and fixed diagonal values
</commit_message>
<xml_diff>
--- a/Aljaz/Naloga1/eurovision_song_contest_2016_2023_matrix.xlsx
+++ b/Aljaz/Naloga1/eurovision_song_contest_2016_2023_matrix.xlsx
@@ -740,9 +740,7 @@
           <t>Albania</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
         <v>0.6666666666666666</v>
       </c>
@@ -876,9 +874,7 @@
       <c r="B5" t="n">
         <v>0</v>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
         <v>0.2</v>
       </c>
@@ -1012,9 +1008,7 @@
       <c r="C6" t="n">
         <v>0</v>
       </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
         <v>2.5</v>
       </c>
@@ -1148,9 +1142,7 @@
       <c r="D7" t="n">
         <v>1.2</v>
       </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
         <v>0.2</v>
       </c>
@@ -1284,9 +1276,7 @@
       <c r="E8" t="n">
         <v>0</v>
       </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
         <v>2.5</v>
       </c>
@@ -1420,9 +1410,7 @@
       <c r="F9" t="n">
         <v>4.666666666666667</v>
       </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
         <v>3</v>
       </c>
@@ -1556,9 +1544,7 @@
       <c r="G10" t="n">
         <v>0</v>
       </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
         <v>3.25</v>
       </c>
@@ -1825,9 +1811,7 @@
       <c r="H12" t="n">
         <v>1</v>
       </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="n">
         <v>0.5</v>
       </c>
@@ -1961,9 +1945,7 @@
       <c r="I13" t="n">
         <v>2.5</v>
       </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
+      <c r="J13" t="inlineStr"/>
       <c r="K13" t="n">
         <v>1.6</v>
       </c>
@@ -2097,9 +2079,7 @@
       <c r="J14" t="n">
         <v>0</v>
       </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="n">
         <v>2</v>
       </c>
@@ -2233,9 +2213,7 @@
       <c r="K15" t="n">
         <v>1.6</v>
       </c>
-      <c r="L15" t="n">
-        <v>0</v>
-      </c>
+      <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
         <v>2.333333333333333</v>
       </c>
@@ -2369,9 +2347,7 @@
       <c r="L16" t="n">
         <v>1.5</v>
       </c>
-      <c r="M16" t="n">
-        <v>0</v>
-      </c>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="n">
         <v>3.666666666666667</v>
       </c>
@@ -2505,9 +2481,7 @@
       <c r="M17" t="n">
         <v>4.666666666666667</v>
       </c>
-      <c r="N17" t="n">
-        <v>0</v>
-      </c>
+      <c r="N17" t="inlineStr"/>
       <c r="O17" t="n">
         <v>10.5</v>
       </c>
@@ -2641,9 +2615,7 @@
       <c r="N18" t="n">
         <v>9</v>
       </c>
-      <c r="O18" t="n">
-        <v>0</v>
-      </c>
+      <c r="O18" t="inlineStr"/>
       <c r="P18" t="n">
         <v>2.5</v>
       </c>
@@ -2777,9 +2749,7 @@
       <c r="O19" t="n">
         <v>1.75</v>
       </c>
-      <c r="P19" t="n">
-        <v>0</v>
-      </c>
+      <c r="P19" t="inlineStr"/>
       <c r="Q19" t="n">
         <v>0</v>
       </c>
@@ -2913,9 +2883,7 @@
       <c r="P20" t="n">
         <v>2</v>
       </c>
-      <c r="Q20" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q20" t="inlineStr"/>
       <c r="R20" t="n">
         <v>0</v>
       </c>
@@ -3049,9 +3017,7 @@
       <c r="Q21" t="n">
         <v>0</v>
       </c>
-      <c r="R21" t="n">
-        <v>0</v>
-      </c>
+      <c r="R21" t="inlineStr"/>
       <c r="S21" t="n">
         <v>0</v>
       </c>
@@ -3185,9 +3151,7 @@
       <c r="R22" t="n">
         <v>0.3333333333333333</v>
       </c>
-      <c r="S22" t="n">
-        <v>0</v>
-      </c>
+      <c r="S22" t="inlineStr"/>
       <c r="T22" t="n">
         <v>0.6666666666666666</v>
       </c>
@@ -3321,9 +3285,7 @@
       <c r="S23" t="n">
         <v>0</v>
       </c>
-      <c r="T23" t="n">
-        <v>0</v>
-      </c>
+      <c r="T23" t="inlineStr"/>
       <c r="U23" t="n">
         <v>12</v>
       </c>
@@ -3457,9 +3419,7 @@
       <c r="T24" t="n">
         <v>0.6666666666666666</v>
       </c>
-      <c r="U24" t="n">
-        <v>0</v>
-      </c>
+      <c r="U24" t="inlineStr"/>
       <c r="V24" t="n">
         <v>0</v>
       </c>
@@ -3593,9 +3553,7 @@
       <c r="U25" t="n">
         <v>5.333333333333333</v>
       </c>
-      <c r="V25" t="n">
-        <v>0</v>
-      </c>
+      <c r="V25" t="inlineStr"/>
       <c r="W25" t="n">
         <v>1.166666666666667</v>
       </c>
@@ -3729,9 +3687,7 @@
       <c r="V26" t="n">
         <v>0</v>
       </c>
-      <c r="W26" t="n">
-        <v>0</v>
-      </c>
+      <c r="W26" t="inlineStr"/>
       <c r="X26" t="n">
         <v>5.428571428571429</v>
       </c>
@@ -3865,9 +3821,7 @@
       <c r="W27" t="n">
         <v>2</v>
       </c>
-      <c r="X27" t="n">
-        <v>0</v>
-      </c>
+      <c r="X27" t="inlineStr"/>
       <c r="Y27" t="n">
         <v>0</v>
       </c>
@@ -4001,9 +3955,7 @@
       <c r="X28" t="n">
         <v>3.166666666666667</v>
       </c>
-      <c r="Y28" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y28" t="inlineStr"/>
       <c r="Z28" t="n">
         <v>10.4</v>
       </c>
@@ -4137,9 +4089,7 @@
       <c r="Y29" t="n">
         <v>12</v>
       </c>
-      <c r="Z29" t="n">
-        <v>0</v>
-      </c>
+      <c r="Z29" t="inlineStr"/>
       <c r="AA29" t="n">
         <v>0</v>
       </c>
@@ -4273,9 +4223,7 @@
       <c r="Z30" t="n">
         <v>2.75</v>
       </c>
-      <c r="AA30" t="n">
-        <v>0</v>
-      </c>
+      <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="n">
         <v>0.25</v>
       </c>
@@ -4409,9 +4357,7 @@
       <c r="AA31" t="n">
         <v>0</v>
       </c>
-      <c r="AB31" t="n">
-        <v>0</v>
-      </c>
+      <c r="AB31" t="inlineStr"/>
       <c r="AC31" t="n">
         <v>1</v>
       </c>
@@ -4678,9 +4624,7 @@
       <c r="AB33" t="n">
         <v>3.75</v>
       </c>
-      <c r="AC33" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC33" t="inlineStr"/>
       <c r="AD33" t="n">
         <v>1</v>
       </c>
@@ -4814,9 +4758,7 @@
       <c r="AC34" t="n">
         <v>1.166666666666667</v>
       </c>
-      <c r="AD34" t="n">
-        <v>0</v>
-      </c>
+      <c r="AD34" t="inlineStr"/>
       <c r="AE34" t="n">
         <v>1.4</v>
       </c>
@@ -4950,9 +4892,7 @@
       <c r="AD35" t="n">
         <v>0</v>
       </c>
-      <c r="AE35" t="n">
-        <v>0</v>
-      </c>
+      <c r="AE35" t="inlineStr"/>
       <c r="AF35" t="n">
         <v>6</v>
       </c>
@@ -5086,9 +5026,7 @@
       <c r="AE36" t="n">
         <v>3.833333333333333</v>
       </c>
-      <c r="AF36" t="n">
-        <v>0</v>
-      </c>
+      <c r="AF36" t="inlineStr"/>
       <c r="AG36" t="n">
         <v>2.75</v>
       </c>
@@ -5222,9 +5160,7 @@
       <c r="AF37" t="n">
         <v>0</v>
       </c>
-      <c r="AG37" t="n">
-        <v>0</v>
-      </c>
+      <c r="AG37" t="inlineStr"/>
       <c r="AH37" t="n">
         <v>3.5</v>
       </c>
@@ -5358,9 +5294,7 @@
       <c r="AG38" t="n">
         <v>1.75</v>
       </c>
-      <c r="AH38" t="n">
-        <v>0</v>
-      </c>
+      <c r="AH38" t="inlineStr"/>
       <c r="AI38" t="n">
         <v>3.5</v>
       </c>
@@ -5494,9 +5428,7 @@
       <c r="AH39" t="n">
         <v>0</v>
       </c>
-      <c r="AI39" t="n">
-        <v>0</v>
-      </c>
+      <c r="AI39" t="inlineStr"/>
       <c r="AJ39" t="n">
         <v>0</v>
       </c>
@@ -5630,9 +5562,7 @@
       <c r="AI40" t="n">
         <v>7.666666666666667</v>
       </c>
-      <c r="AJ40" t="n">
-        <v>0</v>
-      </c>
+      <c r="AJ40" t="inlineStr"/>
       <c r="AK40" t="n">
         <v>1.6</v>
       </c>
@@ -5766,9 +5696,7 @@
       <c r="AJ41" t="n">
         <v>0.5</v>
       </c>
-      <c r="AK41" t="n">
-        <v>0</v>
-      </c>
+      <c r="AK41" t="inlineStr"/>
       <c r="AL41" t="n">
         <v>8.666666666666666</v>
       </c>
@@ -5902,9 +5830,7 @@
       <c r="AK42" t="n">
         <v>10.66666666666667</v>
       </c>
-      <c r="AL42" t="n">
-        <v>0</v>
-      </c>
+      <c r="AL42" t="inlineStr"/>
       <c r="AM42" t="n">
         <v>0.6666666666666666</v>
       </c>
@@ -6038,9 +5964,7 @@
       <c r="AL43" t="n">
         <v>0</v>
       </c>
-      <c r="AM43" t="n">
-        <v>0</v>
-      </c>
+      <c r="AM43" t="inlineStr"/>
       <c r="AN43" t="n">
         <v>3.285714285714286</v>
       </c>
@@ -6174,9 +6098,7 @@
       <c r="AM44" t="n">
         <v>0.5</v>
       </c>
-      <c r="AN44" t="n">
-        <v>0</v>
-      </c>
+      <c r="AN44" t="inlineStr"/>
       <c r="AO44" t="n">
         <v>3.5</v>
       </c>
@@ -6310,9 +6232,7 @@
       <c r="AN45" t="n">
         <v>2.285714285714286</v>
       </c>
-      <c r="AO45" t="n">
-        <v>0</v>
-      </c>
+      <c r="AO45" t="inlineStr"/>
       <c r="AP45" t="n">
         <v>3.2</v>
       </c>
@@ -6446,9 +6366,7 @@
       <c r="AO46" t="n">
         <v>3.5</v>
       </c>
-      <c r="AP46" t="n">
-        <v>0</v>
-      </c>
+      <c r="AP46" t="inlineStr"/>
       <c r="AQ46" t="n">
         <v>2</v>
       </c>
@@ -6582,9 +6500,7 @@
       <c r="AP47" t="n">
         <v>4.166666666666667</v>
       </c>
-      <c r="AQ47" t="n">
-        <v>0</v>
-      </c>
+      <c r="AQ47" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>